<commit_message>
Added Assembler for 1 & 2 operands
</commit_message>
<xml_diff>
--- a/Design/OPCODES.xlsx
+++ b/Design/OPCODES.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamel\Desktop\Spring 2020\Architecture\Project\Harvard_Arch_Processor\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KIMO/Desktop/Harvard_Arch_Processor/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E5826-7B0F-CF43-9B70-98588202EBF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25596" yWindow="0" windowWidth="25596" windowHeight="14400" activeTab="1"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="13940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="296">
   <si>
     <t>0x000</t>
   </si>
@@ -910,12 +911,15 @@
   </si>
   <si>
     <t>0x0/0x000/0x1/0x0/0x0</t>
+  </si>
+  <si>
+    <t>XX0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1365,7 +1369,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K78"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
@@ -1373,22 +1377,22 @@
       <selection pane="bottomLeft" activeCell="G29" sqref="A1:G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
     <col min="7" max="7" width="84.6640625" customWidth="1"/>
     <col min="8" max="8" width="53.33203125" customWidth="1"/>
-    <col min="9" max="9" width="53.44140625" customWidth="1"/>
+    <col min="9" max="9" width="53.5" customWidth="1"/>
     <col min="10" max="10" width="102.6640625" customWidth="1"/>
     <col min="11" max="11" width="69.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>46</v>
       </c>
@@ -1423,7 +1427,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1450,7 +1454,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1477,7 +1481,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1533,7 +1537,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1562,7 +1566,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -1591,7 +1595,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1620,7 +1624,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1651,7 +1655,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1684,7 +1688,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1717,7 +1721,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1750,7 +1754,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1783,7 +1787,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1845,7 +1849,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1878,7 +1882,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1907,7 +1911,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1936,7 +1940,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1965,7 +1969,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1992,7 +1996,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -2019,7 +2023,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -2077,7 +2081,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -2106,7 +2110,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -2135,7 +2139,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2199,7 +2203,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -2234,7 +2238,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -2269,7 +2273,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2279,7 +2283,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>65</v>
       </c>
@@ -2300,7 +2304,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>63</v>
       </c>
@@ -2329,7 +2333,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
@@ -2358,7 +2362,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>54</v>
       </c>
@@ -2387,7 +2391,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>55</v>
       </c>
@@ -2416,7 +2420,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>56</v>
       </c>
@@ -2441,7 +2445,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>57</v>
       </c>
@@ -2468,7 +2472,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>58</v>
       </c>
@@ -2497,7 +2501,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
@@ -2526,7 +2530,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>60</v>
       </c>
@@ -2553,7 +2557,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>61</v>
       </c>
@@ -2578,7 +2582,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>62</v>
       </c>
@@ -2607,7 +2611,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>80</v>
       </c>
@@ -2634,7 +2638,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>107</v>
       </c>
@@ -2657,7 +2661,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>108</v>
       </c>
@@ -2686,7 +2690,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>109</v>
       </c>
@@ -2713,7 +2717,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>125</v>
       </c>
@@ -2736,7 +2740,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>126</v>
       </c>
@@ -2765,7 +2769,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>127</v>
       </c>
@@ -2792,7 +2796,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
         <v>144</v>
       </c>
@@ -2813,7 +2817,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>145</v>
       </c>
@@ -2838,7 +2842,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>126</v>
       </c>
@@ -2859,7 +2863,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>139</v>
       </c>
@@ -2876,7 +2880,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>111</v>
       </c>
@@ -2904,7 +2908,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>140</v>
       </c>
@@ -2933,7 +2937,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>141</v>
       </c>
@@ -2962,7 +2966,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>143</v>
       </c>
@@ -2991,7 +2995,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
@@ -3016,7 +3020,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3029,7 +3033,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3042,7 +3046,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3055,7 +3059,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3068,7 +3072,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3081,7 +3085,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3094,7 +3098,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3107,7 +3111,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3120,7 +3124,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3133,7 +3137,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3146,7 +3150,7 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3159,7 +3163,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3172,7 +3176,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3185,7 +3189,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3198,7 +3202,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3211,7 +3215,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3224,7 +3228,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3237,7 +3241,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3250,7 +3254,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3263,7 +3267,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3278,17 +3282,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E40:F40"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="E43:F43"/>
@@ -3301,6 +3294,17 @@
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="G47:H47"/>
     <mergeCell ref="C53:G53"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3308,31 +3312,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="162" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
     <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
     <col min="7" max="7" width="33.6640625" customWidth="1"/>
-    <col min="8" max="8" width="42.77734375" customWidth="1"/>
+    <col min="8" max="8" width="42.83203125" customWidth="1"/>
     <col min="9" max="9" width="65.6640625" customWidth="1"/>
-    <col min="10" max="10" width="64.77734375" customWidth="1"/>
-    <col min="11" max="11" width="56.77734375" customWidth="1"/>
+    <col min="10" max="10" width="64.83203125" customWidth="1"/>
+    <col min="11" max="11" width="56.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>46</v>
       </c>
@@ -3367,7 +3371,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
@@ -3394,7 +3398,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -3421,7 +3425,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
@@ -3448,7 +3452,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
@@ -3477,7 +3481,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
@@ -3506,7 +3510,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>48</v>
       </c>
@@ -3535,7 +3539,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
@@ -3564,7 +3568,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>10</v>
       </c>
@@ -3595,7 +3599,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
@@ -3628,7 +3632,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>12</v>
       </c>
@@ -3661,7 +3665,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>13</v>
       </c>
@@ -3694,7 +3698,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
@@ -3727,7 +3731,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>5</v>
       </c>
@@ -3756,7 +3760,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>15</v>
       </c>
@@ -3770,7 +3774,7 @@
         <v>40</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>41</v>
+        <v>295</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>40</v>
@@ -3789,7 +3793,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>16</v>
       </c>
@@ -3803,7 +3807,7 @@
         <v>40</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>41</v>
+        <v>295</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>40</v>
@@ -3822,7 +3826,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>28</v>
       </c>
@@ -3851,7 +3855,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>29</v>
       </c>
@@ -3880,7 +3884,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>34</v>
       </c>
@@ -3909,7 +3913,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>35</v>
       </c>
@@ -3936,7 +3940,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>36</v>
       </c>
@@ -3963,7 +3967,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>30</v>
       </c>
@@ -3992,7 +3996,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>31</v>
       </c>
@@ -4021,7 +4025,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>32</v>
       </c>
@@ -4050,7 +4054,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>33</v>
       </c>
@@ -4079,7 +4083,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>24</v>
       </c>
@@ -4112,7 +4116,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>25</v>
       </c>
@@ -4143,7 +4147,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>26</v>
       </c>
@@ -4178,7 +4182,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>27</v>
       </c>
@@ -4211,25 +4215,25 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="H33" s="12" t="s">
         <v>193</v>
       </c>
@@ -4243,7 +4247,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>182</v>
       </c>
@@ -4263,7 +4267,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -4283,7 +4287,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>216</v>
       </c>
@@ -4303,7 +4307,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>217</v>
       </c>
@@ -4318,7 +4322,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H38" s="1" t="s">
         <v>200</v>
       </c>
@@ -4330,7 +4334,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H39" s="1" t="s">
         <v>201</v>
       </c>
@@ -4342,7 +4346,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H40" s="9" t="s">
         <v>202</v>
       </c>
@@ -4356,7 +4360,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H41" s="7" t="s">
         <v>200</v>
       </c>
@@ -4370,7 +4374,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H42" s="7" t="s">
         <v>203</v>
       </c>
@@ -4384,7 +4388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
         <v>209</v>
@@ -4396,7 +4400,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
         <v>210</v>
@@ -4408,7 +4412,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H45" s="1"/>
       <c r="I45" s="9" t="s">
         <v>212</v>
@@ -4420,7 +4424,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H46" s="1"/>
       <c r="I46" s="7" t="s">
         <v>213</v>
@@ -4430,7 +4434,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H47" s="1"/>
       <c r="I47" s="7" t="s">
         <v>214</v>
@@ -4440,7 +4444,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H48" s="1"/>
       <c r="I48" s="9" t="s">
         <v>234</v>
@@ -4448,7 +4452,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H49" s="1"/>
       <c r="I49" s="1" t="s">
         <v>235</v>
@@ -4458,7 +4462,7 @@
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
         <v>236</v>
@@ -4468,7 +4472,7 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H51" s="1"/>
       <c r="I51" s="9" t="s">
         <v>237</v>
@@ -4478,7 +4482,7 @@
       </c>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
         <v>238</v>
@@ -4488,7 +4492,7 @@
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
         <v>239</v>
@@ -4498,7 +4502,7 @@
       </c>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H54" s="1"/>
       <c r="I54" s="1" t="s">
         <v>241</v>
@@ -4508,7 +4512,7 @@
       </c>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H55" s="1"/>
       <c r="I55" s="1" t="s">
         <v>243</v>
@@ -4516,7 +4520,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
         <v>245</v>
@@ -4524,7 +4528,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H57" s="1"/>
       <c r="I57" s="1" t="s">
         <v>246</v>
@@ -4532,7 +4536,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
         <v>247</v>
@@ -4540,7 +4544,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H59" s="1"/>
       <c r="I59" s="1" t="s">
         <v>248</v>
@@ -4548,22 +4552,22 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="8:11" x14ac:dyDescent="0.2">
       <c r="I60" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="8:11" x14ac:dyDescent="0.2">
       <c r="I61" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="62" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="8:11" x14ac:dyDescent="0.2">
       <c r="I62" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="63" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="8:11" x14ac:dyDescent="0.2">
       <c r="I63" s="1" t="s">
         <v>277</v>
       </c>

</xml_diff>

<commit_message>
missing INT + RTI
</commit_message>
<xml_diff>
--- a/Design/OPCODES.xlsx
+++ b/Design/OPCODES.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="301">
   <si>
     <t>0x000</t>
   </si>
@@ -925,6 +925,9 @@
   </si>
   <si>
     <t>0x1/0x001/0x1/0x0/0x0/0x1</t>
+  </si>
+  <si>
+    <t>0x0/0x00/0x0/0x1</t>
   </si>
 </sst>
 </file>
@@ -3293,17 +3296,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E40:F40"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="E43:F43"/>
@@ -3316,6 +3308,17 @@
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="G47:H47"/>
     <mergeCell ref="C53:G53"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3326,10 +3329,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3975,7 +3978,7 @@
         <v>296</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>257</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>